<commit_message>
Almost done with day2
</commit_message>
<xml_diff>
--- a/ExcelEsport/Day2.xlsx
+++ b/ExcelEsport/Day2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/ExcelEsport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{C601C728-F637-45EB-B04B-628417EDA732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B26EAD4-9F8B-4162-9701-5444B73C74B3}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="8_{C601C728-F637-45EB-B04B-628417EDA732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B750006-DCF9-46EA-B882-5308B3CFB06A}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>FROM:</t>
   </si>
@@ -202,12 +202,30 @@
   </si>
   <si>
     <t>EXACT</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Geography Problem</t>
+  </si>
+  <si>
+    <t>Flagstaff, Arizona|Boulder, Colorado|Chicago, Illinois|Tempe, Arizona|Newport, Rhode Island|Ortando, Florida|Tuscaloosa, Alabama|Orem,Utah| Quezon City, Philippines| Columbus, Ohio|Bloomington, Indiana|Montreal, Quebec|Antananarivo, Madagascar|Perth, Australia| Hong Kong| Fairfield, Iowa| Reutlingen, Germany| Edmond, Oklahoma| Warsaw, Poland| Durham, North Carolina| Dekalb, Illinois| Milan, Italy</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;\-0;0;@"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -466,15 +484,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="17"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
@@ -778,15 +796,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>26670</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>59942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>511570</xdr:colOff>
+      <xdr:colOff>205740</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>34333</xdr:rowOff>
+      <xdr:rowOff>34334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -809,8 +827,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3076575" y="2847975"/>
-          <a:ext cx="7392430" cy="301033"/>
+          <a:off x="3074670" y="2831717"/>
+          <a:ext cx="7717155" cy="317292"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>282150</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>57803</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F415469-A7A7-E968-E460-95C3AF971766}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="32089725"/>
+          <a:ext cx="1505160" cy="4677428"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -869,6 +931,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -950,7 +1016,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1242,18 +1308,19 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1329,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1270,8 +1337,11 @@
         <v>27</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F2" s="17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1280,17 +1350,17 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1299,12 +1369,12 @@
         <v>?senihs wodniw rednoy hguorht thgil tahw ,tfoS</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -1315,59 +1385,59 @@
       </c>
     </row>
     <row r="19" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="F19" s="18" t="str">
+      <c r="F19" s="16" t="str">
         <f>_xlfn.CONCAT(H27:H66)</f>
         <v>⚂⚃⚀⚅⚂⚂⚂⚁⚁⚂⚃⚂⚃⚃⚄⚀⚄⚁⚁⚀⚃⚂⚅⚃⚁⚅⚅⚀⚃⚅⚅⚀⚃⚁⚃⚁⚁⚂⚄⚃</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B24" s="16">
+      <c r="B24" s="18">
         <v>1</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="14" t="s">
         <v>40</v>
       </c>
       <c r="K24">
         <f>LEN(F24)</f>
         <v>40</v>
       </c>
-      <c r="N24" s="17" t="str" cm="1">
+      <c r="N24" s="15" t="str" cm="1">
         <f t="array" ref="N24:N43">MID(F19,_xlfn.SEQUENCE(LEN(F19)/2,1,1,2),2)</f>
         <v>⚂⚃</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B25" s="16">
+      <c r="B25" s="18">
         <v>2</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="N25" s="17" t="str">
+      <c r="N25" s="15" t="str">
         <v>⚀⚅</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B26" s="16">
+      <c r="B26" s="18">
         <v>4</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="N26" s="17" t="str">
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="N26" s="15" t="str">
         <v>⚂⚂</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B27" s="16">
+      <c r="B27" s="18">
         <v>3</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G27">
@@ -1377,15 +1447,15 @@
         <f>_xlfn.XLOOKUP(G27,$B$24:$B$29,$C$24:$C$29)</f>
         <v>⚂</v>
       </c>
-      <c r="N27" s="17" t="str">
+      <c r="N27" s="15" t="str">
         <v>⚂⚁</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B28" s="16">
+      <c r="B28" s="18">
         <v>5</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G28">
@@ -1395,15 +1465,15 @@
         <f t="shared" ref="H28:H66" si="0">_xlfn.XLOOKUP(G28,$B$24:$B$29,$C$24:$C$29)</f>
         <v>⚃</v>
       </c>
-      <c r="N28" s="17" t="str">
+      <c r="N28" s="15" t="str">
         <v>⚁⚂</v>
       </c>
     </row>
     <row r="29" spans="2:14" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B29" s="16">
+      <c r="B29" s="18">
         <v>6</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>35</v>
       </c>
       <c r="G29">
@@ -1413,7 +1483,7 @@
         <f t="shared" si="0"/>
         <v>⚀</v>
       </c>
-      <c r="N29" s="17" t="str">
+      <c r="N29" s="15" t="str">
         <v>⚃⚂</v>
       </c>
     </row>
@@ -1425,7 +1495,7 @@
         <f t="shared" si="0"/>
         <v>⚅</v>
       </c>
-      <c r="N30" s="17" t="str">
+      <c r="N30" s="15" t="str">
         <v>⚃⚃</v>
       </c>
     </row>
@@ -1437,7 +1507,7 @@
         <f t="shared" si="0"/>
         <v>⚂</v>
       </c>
-      <c r="N31" s="17" t="str">
+      <c r="N31" s="15" t="str">
         <v>⚄⚀</v>
       </c>
     </row>
@@ -1449,7 +1519,7 @@
         <f t="shared" si="0"/>
         <v>⚂</v>
       </c>
-      <c r="N32" s="17" t="str">
+      <c r="N32" s="15" t="str">
         <v>⚄⚁</v>
       </c>
     </row>
@@ -1461,7 +1531,7 @@
         <f t="shared" si="0"/>
         <v>⚂</v>
       </c>
-      <c r="N33" s="17" t="str">
+      <c r="N33" s="15" t="str">
         <v>⚁⚀</v>
       </c>
     </row>
@@ -1473,7 +1543,7 @@
         <f t="shared" si="0"/>
         <v>⚁</v>
       </c>
-      <c r="N34" s="17" t="str">
+      <c r="N34" s="15" t="str">
         <v>⚃⚂</v>
       </c>
     </row>
@@ -1485,7 +1555,7 @@
         <f t="shared" si="0"/>
         <v>⚁</v>
       </c>
-      <c r="N35" s="17" t="str">
+      <c r="N35" s="15" t="str">
         <v>⚅⚃</v>
       </c>
     </row>
@@ -1497,7 +1567,7 @@
         <f t="shared" si="0"/>
         <v>⚂</v>
       </c>
-      <c r="N36" s="17" t="str">
+      <c r="N36" s="15" t="str">
         <v>⚁⚅</v>
       </c>
     </row>
@@ -1509,7 +1579,7 @@
         <f t="shared" si="0"/>
         <v>⚃</v>
       </c>
-      <c r="N37" s="17" t="str">
+      <c r="N37" s="15" t="str">
         <v>⚅⚀</v>
       </c>
     </row>
@@ -1521,7 +1591,7 @@
         <f t="shared" si="0"/>
         <v>⚂</v>
       </c>
-      <c r="N38" s="17" t="str">
+      <c r="N38" s="15" t="str">
         <v>⚃⚅</v>
       </c>
     </row>
@@ -1533,7 +1603,7 @@
         <f t="shared" si="0"/>
         <v>⚃</v>
       </c>
-      <c r="N39" s="17" t="str">
+      <c r="N39" s="15" t="str">
         <v>⚅⚀</v>
       </c>
     </row>
@@ -1545,7 +1615,7 @@
         <f t="shared" si="0"/>
         <v>⚃</v>
       </c>
-      <c r="N40" s="17" t="str">
+      <c r="N40" s="15" t="str">
         <v>⚃⚁</v>
       </c>
     </row>
@@ -1557,7 +1627,7 @@
         <f t="shared" si="0"/>
         <v>⚄</v>
       </c>
-      <c r="N41" s="17" t="str">
+      <c r="N41" s="15" t="str">
         <v>⚃⚁</v>
       </c>
     </row>
@@ -1569,7 +1639,7 @@
         <f t="shared" si="0"/>
         <v>⚀</v>
       </c>
-      <c r="N42" s="17" t="str">
+      <c r="N42" s="15" t="str">
         <v>⚁⚂</v>
       </c>
     </row>
@@ -1581,7 +1651,7 @@
         <f t="shared" si="0"/>
         <v>⚄</v>
       </c>
-      <c r="N43" s="17" t="str">
+      <c r="N43" s="15" t="str">
         <v>⚄⚃</v>
       </c>
     </row>
@@ -1798,53 +1868,53 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B70" s="17" t="str" cm="1">
+      <c r="B70" s="15" t="str" cm="1">
         <f t="array" ref="B70:B79">MID(F19,_xlfn.SEQUENCE(LEN(F19)/4,,4,4),1)</f>
         <v>⚅</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B71" s="17" t="str">
+      <c r="B71" s="15" t="str">
         <v>⚁</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B72" s="17" t="str">
+      <c r="B72" s="15" t="str">
         <v>⚂</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B73" s="17" t="str">
+      <c r="B73" s="15" t="str">
         <v>⚀</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B74" s="17" t="str">
+      <c r="B74" s="15" t="str">
         <v>⚀</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B75" s="17" t="str">
+      <c r="B75" s="15" t="str">
         <v>⚃</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B76" s="17" t="str">
+      <c r="B76" s="15" t="str">
         <v>⚀</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B77" s="17" t="str">
+      <c r="B77" s="15" t="str">
         <v>⚀</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B78" s="17" t="str">
+      <c r="B78" s="15" t="str">
         <v>⚁</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="B79" s="17" t="str">
+      <c r="B79" s="15" t="str">
         <v>⚃</v>
       </c>
     </row>
@@ -1865,7 +1935,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A84" s="17" t="str" cm="1">
+      <c r="A84" s="15" t="str" cm="1">
         <f t="array" ref="A84:A121">MID(F19,_xlfn.SEQUENCE(LEN(F19)-2,1,1,1),3)</f>
         <v>⚂⚃⚀</v>
       </c>
@@ -1891,7 +1961,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A85" s="17" t="str">
+      <c r="A85" s="15" t="str">
         <v>⚃⚀⚅</v>
       </c>
       <c r="B85" t="b">
@@ -1900,7 +1970,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A86" s="17" t="str">
+      <c r="A86" s="15" t="str">
         <v>⚀⚅⚂</v>
       </c>
       <c r="B86" t="b">
@@ -1909,7 +1979,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A87" s="17" t="str">
+      <c r="A87" s="15" t="str">
         <v>⚅⚂⚂</v>
       </c>
       <c r="B87" t="b">
@@ -1918,7 +1988,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A88" s="17" t="str">
+      <c r="A88" s="15" t="str">
         <v>⚂⚂⚂</v>
       </c>
       <c r="B88" t="b">
@@ -1927,7 +1997,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A89" s="17" t="str">
+      <c r="A89" s="15" t="str">
         <v>⚂⚂⚁</v>
       </c>
       <c r="B89" t="b">
@@ -1936,7 +2006,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A90" s="17" t="str">
+      <c r="A90" s="15" t="str">
         <v>⚂⚁⚁</v>
       </c>
       <c r="B90" t="b">
@@ -1945,7 +2015,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A91" s="17" t="str">
+      <c r="A91" s="15" t="str">
         <v>⚁⚁⚂</v>
       </c>
       <c r="B91" t="b">
@@ -1954,7 +2024,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A92" s="17" t="str">
+      <c r="A92" s="15" t="str">
         <v>⚁⚂⚃</v>
       </c>
       <c r="B92" t="b">
@@ -1963,7 +2033,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A93" s="17" t="str">
+      <c r="A93" s="15" t="str">
         <v>⚂⚃⚂</v>
       </c>
       <c r="B93" t="b">
@@ -1972,7 +2042,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A94" s="17" t="str">
+      <c r="A94" s="15" t="str">
         <v>⚃⚂⚃</v>
       </c>
       <c r="B94" t="b">
@@ -1981,7 +2051,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A95" s="17" t="str">
+      <c r="A95" s="15" t="str">
         <v>⚂⚃⚃</v>
       </c>
       <c r="B95" t="b">
@@ -1990,7 +2060,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A96" s="17" t="str">
+      <c r="A96" s="15" t="str">
         <v>⚃⚃⚄</v>
       </c>
       <c r="B96" t="b">
@@ -1999,7 +2069,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A97" s="17" t="str">
+      <c r="A97" s="15" t="str">
         <v>⚃⚄⚀</v>
       </c>
       <c r="B97" t="b">
@@ -2008,7 +2078,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A98" s="17" t="str">
+      <c r="A98" s="15" t="str">
         <v>⚄⚀⚄</v>
       </c>
       <c r="B98" t="b">
@@ -2017,7 +2087,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A99" s="17" t="str">
+      <c r="A99" s="15" t="str">
         <v>⚀⚄⚁</v>
       </c>
       <c r="B99" t="b">
@@ -2026,7 +2096,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A100" s="17" t="str">
+      <c r="A100" s="15" t="str">
         <v>⚄⚁⚁</v>
       </c>
       <c r="B100" t="b">
@@ -2035,7 +2105,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A101" s="17" t="str">
+      <c r="A101" s="15" t="str">
         <v>⚁⚁⚀</v>
       </c>
       <c r="B101" t="b">
@@ -2044,7 +2114,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A102" s="17" t="str">
+      <c r="A102" s="15" t="str">
         <v>⚁⚀⚃</v>
       </c>
       <c r="B102" t="b">
@@ -2053,7 +2123,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A103" s="17" t="str">
+      <c r="A103" s="15" t="str">
         <v>⚀⚃⚂</v>
       </c>
       <c r="B103" t="b">
@@ -2062,7 +2132,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A104" s="17" t="str">
+      <c r="A104" s="15" t="str">
         <v>⚃⚂⚅</v>
       </c>
       <c r="B104" t="b">
@@ -2071,7 +2141,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A105" s="17" t="str">
+      <c r="A105" s="15" t="str">
         <v>⚂⚅⚃</v>
       </c>
       <c r="B105" t="b">
@@ -2080,7 +2150,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A106" s="17" t="str">
+      <c r="A106" s="15" t="str">
         <v>⚅⚃⚁</v>
       </c>
       <c r="B106" t="b">
@@ -2089,7 +2159,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A107" s="17" t="str">
+      <c r="A107" s="15" t="str">
         <v>⚃⚁⚅</v>
       </c>
       <c r="B107" t="b">
@@ -2098,7 +2168,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A108" s="17" t="str">
+      <c r="A108" s="15" t="str">
         <v>⚁⚅⚅</v>
       </c>
       <c r="B108" t="b">
@@ -2107,7 +2177,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A109" s="17" t="str">
+      <c r="A109" s="15" t="str">
         <v>⚅⚅⚀</v>
       </c>
       <c r="B109" t="b">
@@ -2116,7 +2186,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A110" s="17" t="str">
+      <c r="A110" s="15" t="str">
         <v>⚅⚀⚃</v>
       </c>
       <c r="B110" t="b">
@@ -2125,7 +2195,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A111" s="17" t="str">
+      <c r="A111" s="15" t="str">
         <v>⚀⚃⚅</v>
       </c>
       <c r="B111" t="b">
@@ -2134,7 +2204,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A112" s="17" t="str">
+      <c r="A112" s="15" t="str">
         <v>⚃⚅⚅</v>
       </c>
       <c r="B112" t="b">
@@ -2142,8 +2212,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A113" s="17" t="str">
+    <row r="113" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A113" s="15" t="str">
         <v>⚅⚅⚀</v>
       </c>
       <c r="B113" t="b">
@@ -2151,8 +2221,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A114" s="17" t="str">
+    <row r="114" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A114" s="15" t="str">
         <v>⚅⚀⚃</v>
       </c>
       <c r="B114" t="b">
@@ -2160,8 +2230,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A115" s="17" t="str">
+    <row r="115" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A115" s="15" t="str">
         <v>⚀⚃⚁</v>
       </c>
       <c r="B115" t="b">
@@ -2169,8 +2239,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A116" s="17" t="str">
+    <row r="116" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A116" s="15" t="str">
         <v>⚃⚁⚃</v>
       </c>
       <c r="B116" t="b">
@@ -2178,8 +2248,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A117" s="17" t="str">
+    <row r="117" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A117" s="15" t="str">
         <v>⚁⚃⚁</v>
       </c>
       <c r="B117" t="b">
@@ -2187,8 +2257,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A118" s="17" t="str">
+    <row r="118" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A118" s="15" t="str">
         <v>⚃⚁⚁</v>
       </c>
       <c r="B118" t="b">
@@ -2196,8 +2266,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A119" s="17" t="str">
+    <row r="119" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A119" s="15" t="str">
         <v>⚁⚁⚂</v>
       </c>
       <c r="B119" t="b">
@@ -2205,8 +2275,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A120" s="17" t="str">
+    <row r="120" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A120" s="15" t="str">
         <v>⚁⚂⚄</v>
       </c>
       <c r="B120" t="b">
@@ -2214,8 +2284,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="24.6" x14ac:dyDescent="0.45">
-      <c r="A121" s="17" t="str">
+    <row r="121" spans="1:8" ht="24.6" x14ac:dyDescent="0.45">
+      <c r="A121" s="15" t="str">
         <v>⚂⚄⚃</v>
       </c>
       <c r="B121" t="b">
@@ -2223,9 +2293,295 @@
         <v>0</v>
       </c>
     </row>
+    <row r="124" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F125" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
+        <v>49</v>
+      </c>
+      <c r="G127" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F128" t="str" cm="1">
+        <f t="array" ref="F128:G149">TRIM(_xlfn.TEXTSPLIT(F125,",","|",TRUE,,""))</f>
+        <v>Flagstaff</v>
+      </c>
+      <c r="G128" t="str">
+        <v>Arizona</v>
+      </c>
+      <c r="H128" t="str" cm="1">
+        <f t="array" ref="H128">TRIM(_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F128,_xlfn.SEQUENCE(LEN(F128),1,LEN(F128),-1),1))))</f>
+        <v>aaffFglst</v>
+      </c>
+    </row>
+    <row r="129" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F129" t="str">
+        <v>Boulder</v>
+      </c>
+      <c r="G129" t="str">
+        <v>Colorado</v>
+      </c>
+      <c r="H129" t="str" cm="1">
+        <f t="array" ref="H129">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F129,_xlfn.SEQUENCE(LEN(F129),1,LEN(F129),-1),1)))</f>
+        <v>Bdeloru</v>
+      </c>
+    </row>
+    <row r="130" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F130" t="str">
+        <v>Chicago</v>
+      </c>
+      <c r="G130" t="str">
+        <v>Illinois</v>
+      </c>
+      <c r="H130" t="str" cm="1">
+        <f t="array" ref="H130">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F130,_xlfn.SEQUENCE(LEN(F130),1,LEN(F130),-1),1)))</f>
+        <v>acCghio</v>
+      </c>
+    </row>
+    <row r="131" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F131" t="str">
+        <v>Tempe</v>
+      </c>
+      <c r="G131" t="str">
+        <v>Arizona</v>
+      </c>
+      <c r="H131" t="str" cm="1">
+        <f t="array" ref="H131">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F131,_xlfn.SEQUENCE(LEN(F131),1,LEN(F131),-1),1)))</f>
+        <v>eempT</v>
+      </c>
+    </row>
+    <row r="132" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F132" t="str">
+        <v>Newport</v>
+      </c>
+      <c r="G132" t="str">
+        <v>Rhode Island</v>
+      </c>
+      <c r="H132" t="str" cm="1">
+        <f t="array" ref="H132">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F132,_xlfn.SEQUENCE(LEN(F132),1,LEN(F132),-1),1)))</f>
+        <v>eNoprtw</v>
+      </c>
+    </row>
+    <row r="133" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F133" t="str">
+        <v>Ortando</v>
+      </c>
+      <c r="G133" t="str">
+        <v>Florida</v>
+      </c>
+      <c r="H133" t="str" cm="1">
+        <f t="array" ref="H133">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F133,_xlfn.SEQUENCE(LEN(F133),1,LEN(F133),-1),1)))</f>
+        <v>adnoOrt</v>
+      </c>
+    </row>
+    <row r="134" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F134" t="str">
+        <v>Tuscaloosa</v>
+      </c>
+      <c r="G134" t="str">
+        <v>Alabama</v>
+      </c>
+      <c r="H134" t="str" cm="1">
+        <f t="array" ref="H134">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F134,_xlfn.SEQUENCE(LEN(F134),1,LEN(F134),-1),1)))</f>
+        <v>aacloossTu</v>
+      </c>
+    </row>
+    <row r="135" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F135" t="str">
+        <v>Orem</v>
+      </c>
+      <c r="G135" t="str">
+        <v>Utah</v>
+      </c>
+      <c r="H135" t="str" cm="1">
+        <f t="array" ref="H135">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F135,_xlfn.SEQUENCE(LEN(F135),1,LEN(F135),-1),1)))</f>
+        <v>emOr</v>
+      </c>
+    </row>
+    <row r="136" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F136" t="str">
+        <v>Quezon City</v>
+      </c>
+      <c r="G136" t="str">
+        <v>Philippines</v>
+      </c>
+      <c r="H136" t="str" cm="1">
+        <f t="array" ref="H136">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F136,_xlfn.SEQUENCE(LEN(F136),1,LEN(F136),-1),1)))</f>
+        <v xml:space="preserve"> CeinoQtuyz</v>
+      </c>
+    </row>
+    <row r="137" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F137" t="str">
+        <v>Columbus</v>
+      </c>
+      <c r="G137" t="str">
+        <v>Ohio</v>
+      </c>
+      <c r="H137" t="str" cm="1">
+        <f t="array" ref="H137">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F137,_xlfn.SEQUENCE(LEN(F137),1,LEN(F137),-1),1)))</f>
+        <v>bClmosuu</v>
+      </c>
+    </row>
+    <row r="138" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F138" t="str">
+        <v>Bloomington</v>
+      </c>
+      <c r="G138" t="str">
+        <v>Indiana</v>
+      </c>
+      <c r="H138" t="str" cm="1">
+        <f t="array" ref="H138">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F138,_xlfn.SEQUENCE(LEN(F138),1,LEN(F138),-1),1)))</f>
+        <v>Bgilmnnooot</v>
+      </c>
+    </row>
+    <row r="139" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F139" t="str">
+        <v>Montreal</v>
+      </c>
+      <c r="G139" t="str">
+        <v>Quebec</v>
+      </c>
+      <c r="H139" t="str" cm="1">
+        <f t="array" ref="H139">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F139,_xlfn.SEQUENCE(LEN(F139),1,LEN(F139),-1),1)))</f>
+        <v>aelMnort</v>
+      </c>
+    </row>
+    <row r="140" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F140" t="str">
+        <v>Antananarivo</v>
+      </c>
+      <c r="G140" t="str">
+        <v>Madagascar</v>
+      </c>
+      <c r="H140" t="str" cm="1">
+        <f t="array" ref="H140">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F140,_xlfn.SEQUENCE(LEN(F140),1,LEN(F140),-1),1)))</f>
+        <v>aaaAinnnortv</v>
+      </c>
+    </row>
+    <row r="141" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F141" t="str">
+        <v>Perth</v>
+      </c>
+      <c r="G141" t="str">
+        <v>Australia</v>
+      </c>
+      <c r="H141" t="str" cm="1">
+        <f t="array" ref="H141">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F141,_xlfn.SEQUENCE(LEN(F141),1,LEN(F141),-1),1)))</f>
+        <v>ehPrt</v>
+      </c>
+    </row>
+    <row r="142" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F142" t="str">
+        <v>Hong Kong</v>
+      </c>
+      <c r="G142" t="str">
+        <v/>
+      </c>
+      <c r="H142" t="str" cm="1">
+        <f t="array" ref="H142">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F142,_xlfn.SEQUENCE(LEN(F142),1,LEN(F142),-1),1)))</f>
+        <v xml:space="preserve"> ggHKnnoo</v>
+      </c>
+    </row>
+    <row r="143" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F143" t="str">
+        <v>Fairfield</v>
+      </c>
+      <c r="G143" t="str">
+        <v>Iowa</v>
+      </c>
+      <c r="H143" t="str" cm="1">
+        <f t="array" ref="H143">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F143,_xlfn.SEQUENCE(LEN(F143),1,LEN(F143),-1),1)))</f>
+        <v>adefFiilr</v>
+      </c>
+    </row>
+    <row r="144" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F144" t="str">
+        <v>Reutlingen</v>
+      </c>
+      <c r="G144" t="str">
+        <v>Germany</v>
+      </c>
+      <c r="H144" t="str" cm="1">
+        <f t="array" ref="H144">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F144,_xlfn.SEQUENCE(LEN(F144),1,LEN(F144),-1),1)))</f>
+        <v>eegilnnRtu</v>
+      </c>
+    </row>
+    <row r="145" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F145" t="str">
+        <v>Edmond</v>
+      </c>
+      <c r="G145" t="str">
+        <v>Oklahoma</v>
+      </c>
+      <c r="H145" t="str" cm="1">
+        <f t="array" ref="H145">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F145,_xlfn.SEQUENCE(LEN(F145),1,LEN(F145),-1),1)))</f>
+        <v>ddEmno</v>
+      </c>
+    </row>
+    <row r="146" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F146" t="str">
+        <v>Warsaw</v>
+      </c>
+      <c r="G146" t="str">
+        <v>Poland</v>
+      </c>
+      <c r="H146" t="str" cm="1">
+        <f t="array" ref="H146">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F146,_xlfn.SEQUENCE(LEN(F146),1,LEN(F146),-1),1)))</f>
+        <v>aarswW</v>
+      </c>
+    </row>
+    <row r="147" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F147" t="str">
+        <v>Durham</v>
+      </c>
+      <c r="G147" t="str">
+        <v>North Carolina</v>
+      </c>
+      <c r="H147" t="str" cm="1">
+        <f t="array" ref="H147">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F147,_xlfn.SEQUENCE(LEN(F147),1,LEN(F147),-1),1)))</f>
+        <v>aDhmru</v>
+      </c>
+    </row>
+    <row r="148" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F148" t="str">
+        <v>Dekalb</v>
+      </c>
+      <c r="G148" t="str">
+        <v>Illinois</v>
+      </c>
+      <c r="H148" t="str" cm="1">
+        <f t="array" ref="H148">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F148,_xlfn.SEQUENCE(LEN(F148),1,LEN(F148),-1),1)))</f>
+        <v>abDekl</v>
+      </c>
+    </row>
+    <row r="149" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F149" t="str">
+        <v>Milan</v>
+      </c>
+      <c r="G149" t="str">
+        <v>Italy</v>
+      </c>
+      <c r="H149" t="str" cm="1">
+        <f t="array" ref="H149">_xlfn.CONCAT(_xlfn._xlws.SORT(MID(F149,_xlfn.SEQUENCE(LEN(F149),1,LEN(F149),-1),1)))</f>
+        <v>ailMn</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{97AF205F-88AC-466D-B639-275C38AB6731}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2408,19 +2764,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -2428,11 +2780,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -2440,19 +2791,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -2460,11 +2807,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -2472,19 +2818,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -2492,11 +2834,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -2504,13 +2845,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>